<commit_message>
Added treatment episode creation, incidence, prevalence, discontinuation calculation
Need to fix: for datasets with >1 unique ATC, incidence, prevalence and probably are being calculated wrong and need to be looked at.
</commit_message>
<xml_diff>
--- a/DEVELOPMENT/analysis/definitions/codelists/20250515_ADEPT_medicines.xlsx
+++ b/DEVELOPMENT/analysis/definitions/codelists/20250515_ADEPT_medicines.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgamb\Documents\GitHub\ADEPT_obj1\DEVELOPMENT\analysis\definitions\codelists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B615207-DBB5-4C67-B9F4-31D7578BDA40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4410BE6-6226-4410-8705-438B467C9B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MEDICINES_Obj_1&amp;2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="402">
   <si>
     <t>Drug_abbreviation</t>
   </si>
@@ -1224,13 +1224,31 @@
   </si>
   <si>
     <t>N03AB03</t>
+  </si>
+  <si>
+    <t>DP_EPILEPSY</t>
+  </si>
+  <si>
+    <t>Anti-epileptics</t>
+  </si>
+  <si>
+    <t>N03</t>
+  </si>
+  <si>
+    <t>DP_TCA</t>
+  </si>
+  <si>
+    <t>Tricyclic antidepressants (Non-selective monoamine reuptake inhibitors)</t>
+  </si>
+  <si>
+    <t>N06AA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1281,6 +1299,12 @@
       <color rgb="FF242424"/>
       <name val="Aptos Narrow"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Aptos Narrow"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1311,7 +1335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1330,6 +1354,7 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1667,10 +1692,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:D134"/>
+  <dimension ref="A1:D136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55:XFD55"/>
+    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="B142" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2032,7 +2057,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
         <v>393</v>
       </c>
@@ -2043,7 +2068,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>78</v>
       </c>
@@ -2054,7 +2079,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>81</v>
       </c>
@@ -2065,246 +2090,247 @@
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="6" t="s">
+    <row r="36" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="B36" t="s">
+        <v>397</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="D36"/>
+    </row>
+    <row r="37" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B37" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C37" s="6" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="6" t="s">
+    <row r="38" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
         <v>84</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
+    <row r="39" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B40" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C40" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
+    <row r="41" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B41" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C41" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
+    <row r="42" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B42" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C42" s="6" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
+    <row r="43" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B43" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C43" s="6" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="6" t="s">
+    <row r="44" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B44" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C44" s="6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="6" t="s">
+    <row r="45" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B45" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C45" s="6" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="6" t="s">
+    <row r="46" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B46" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C46" s="6" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="6" t="s">
+    <row r="47" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B47" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C47" s="6" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="47" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
+    <row r="48" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B48" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C48" s="4" t="s">
         <v>389</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>124</v>
+        <v>120</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>121</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="51" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>124</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="52" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="55" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B56" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C56" s="6" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="56" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="4" t="s">
+    <row r="57" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B57" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="C57" s="6" t="s">
         <v>158</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="58" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2320,850 +2346,884 @@
     </row>
     <row r="59" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="60" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="61" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B62" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C62" s="6" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="62" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="4" t="s">
+    <row r="63" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B63" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C63" s="6" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="63" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="6" t="s">
+    <row r="64" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B64" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C64" s="6" t="s">
         <v>197</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="4" t="s">
-        <v>354</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="65" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
-        <v>180</v>
+        <v>354</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>182</v>
+        <v>355</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="66" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="67" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="68" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B69" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="C69" s="4" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="69" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="6" t="s">
+    <row r="70" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B70" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="C70" s="4" t="s">
         <v>365</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>352</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="71" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
-        <v>327</v>
+        <v>351</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>328</v>
+        <v>352</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>329</v>
+        <v>353</v>
       </c>
     </row>
     <row r="72" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B73" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C73" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="73" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="6" t="s">
+    <row r="74" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B74" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C73" s="6" t="s">
+      <c r="C74" s="6" t="s">
         <v>203</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="4" t="s">
-        <v>336</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="75" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B76" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="C75" s="4" t="s">
+      <c r="C76" s="4" t="s">
         <v>383</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="77" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>193</v>
+        <v>189</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>190</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="78" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="6" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
     </row>
     <row r="79" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="80" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="81" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="B81" s="6" t="s">
+      <c r="B82" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="C81" s="6" t="s">
+      <c r="C82" s="6" t="s">
         <v>161</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="83" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B84" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="C83" s="4" t="s">
+      <c r="C84" s="4" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="84" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="6" t="s">
+    <row r="85" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B85" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C84" s="6" t="s">
+      <c r="C85" s="6" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="C85" s="4" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="86" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B87" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="C86" s="4" t="s">
+      <c r="C87" s="4" t="s">
         <v>386</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="C87" s="4" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="88" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B89" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="C88" s="6" t="s">
+      <c r="C89" s="6" t="s">
         <v>317</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="4" t="s">
-        <v>369</v>
-      </c>
-      <c r="B89" s="4" t="s">
-        <v>370</v>
-      </c>
-      <c r="C89" s="4" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="90" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
-        <v>318</v>
+        <v>369</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>319</v>
+        <v>370</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>320</v>
+        <v>371</v>
       </c>
     </row>
     <row r="91" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B92" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="C91" s="4" t="s">
+      <c r="C92" s="4" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="92" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="6" t="s">
+    <row r="93" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B93" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C92" s="6" t="s">
+      <c r="C93" s="6" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="C93" s="4" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="94" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B95" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C94" s="6" t="s">
+      <c r="C95" s="6" t="s">
         <v>179</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="B95" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="C95" s="4" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="96" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="B96" s="6" t="s">
+      <c r="B97" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="C96" s="6" t="s">
+      <c r="C97" s="6" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="97" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="4" t="s">
+    <row r="98" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B98" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="C97" s="6" t="s">
+      <c r="C98" s="6" t="s">
         <v>218</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="B98" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="C98" s="6" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="99" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="6" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="100" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="101" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="102" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="6" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="103" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="6" t="s">
-        <v>255</v>
+        <v>231</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>257</v>
+        <v>233</v>
       </c>
     </row>
     <row r="104" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="C104" s="6" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B105" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="C104" s="4" t="s">
+      <c r="C105" s="4" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="105" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="4" t="s">
+    <row r="106" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="B106" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C105" s="4" t="s">
+      <c r="C106" s="4" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="B106" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="C106" s="6" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="107" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C107" s="6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="B108" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C107" s="6" t="s">
+      <c r="C108" s="6" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="108" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="4" t="s">
+    <row r="109" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="B109" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="C108" s="4" t="s">
+      <c r="C109" s="4" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="109" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="6" t="s">
+    <row r="110" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="B109" s="4" t="s">
+      <c r="B110" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="C109" s="6" t="s">
+      <c r="C110" s="6" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="110" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="4" t="s">
+    <row r="111" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="B110" s="4" t="s">
+      <c r="B111" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C110" s="6" t="s">
+      <c r="C111" s="6" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="111" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="6" t="s">
+    <row r="112" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="B111" s="4" t="s">
+      <c r="B112" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C111" s="6" t="s">
+      <c r="C112" s="6" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="112" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="4" t="s">
+    <row r="113" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="B112" s="4" t="s">
+      <c r="B113" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="C112" s="6" t="s">
+      <c r="C113" s="6" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="113" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="4" t="s">
+    <row r="114" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="B113" s="4" t="s">
+      <c r="B114" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="C113" s="6" t="s">
+      <c r="C114" s="6" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="114" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="4" t="s">
+    <row r="115" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="B114" s="4" t="s">
+      <c r="B115" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="C114" s="6" t="s">
+      <c r="C115" s="6" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="115" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="4" t="s">
+    <row r="116" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="B115" s="4" t="s">
+      <c r="B116" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="C115" s="6" t="s">
+      <c r="C116" s="6" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="116" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="4" t="s">
+    <row r="117" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="B117" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="C116" s="6" t="s">
+      <c r="C117" s="6" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="117" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="4" t="s">
+    <row r="118" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="B118" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="C117" s="6" t="s">
+      <c r="C118" s="6" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="118" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="6" t="s">
+    <row r="119" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B119" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="C118" s="6" t="s">
+      <c r="C119" s="6" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="119" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="4" t="s">
+    <row r="120" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="B119" s="4" t="s">
+      <c r="B120" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="C119" s="6" t="s">
+      <c r="C120" s="6" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="120" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="4" t="s">
+    <row r="121" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="10" t="s">
+        <v>399</v>
+      </c>
+      <c r="B121" t="s">
+        <v>400</v>
+      </c>
+      <c r="C121" t="s">
+        <v>401</v>
+      </c>
+      <c r="D121"/>
+    </row>
+    <row r="122" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="B120" s="4" t="s">
+      <c r="B122" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="C120" s="4" t="s">
+      <c r="C122" s="4" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="121" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="4" t="s">
+    <row r="123" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="B121" s="4" t="s">
+      <c r="B123" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="C121" s="6" t="s">
+      <c r="C123" s="6" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="122" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="4" t="s">
+    <row r="124" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B122" s="4" t="s">
+      <c r="B124" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="C122" s="4" t="s">
+      <c r="C124" s="4" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="123" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="4" t="s">
+    <row r="125" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="B123" s="4" t="s">
+      <c r="B125" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="C123" s="6" t="s">
+      <c r="C125" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="124" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="4" t="s">
+    <row r="126" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="B124" s="4" t="s">
+      <c r="B126" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="C124" s="4" t="s">
+      <c r="C126" s="4" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="125" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="4" t="s">
+    <row r="127" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="B125" s="4" t="s">
+      <c r="B127" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="C125" s="6" t="s">
+      <c r="C127" s="6" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="126" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="4" t="s">
+    <row r="128" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="B126" s="4" t="s">
+      <c r="B128" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="C126" s="6" t="s">
+      <c r="C128" s="6" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="127" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="6" t="s">
+    <row r="129" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="B127" s="4" t="s">
+      <c r="B129" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="C127" s="6" t="s">
+      <c r="C129" s="6" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="128" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="4" t="s">
+    <row r="130" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="B128" s="4" t="s">
+      <c r="B130" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="C128" s="4" t="s">
+      <c r="C130" s="4" t="s">
         <v>299</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="B129" s="4" t="s">
-        <v>322</v>
-      </c>
-      <c r="C129" s="4" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="B130" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="C130" s="6" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="131" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="C131" s="4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A132" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="C132" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="D132" s="1"/>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A133" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="B131" s="4" t="s">
+      <c r="B133" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="C131" s="4" t="s">
+      <c r="C133" s="4" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A132" s="4" t="s">
+      <c r="D133" s="1"/>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A134" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="B132" s="4" t="s">
+      <c r="B134" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="C132" s="4" t="s">
+      <c r="C134" s="4" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A133" s="6" t="s">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A135" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="B133" s="4" t="s">
+      <c r="B135" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="C133" s="6" t="s">
+      <c r="C135" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="D133" s="1"/>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A134" s="6" t="s">
+      <c r="D135" s="1"/>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A136" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="B134" s="4" t="s">
+      <c r="B136" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="C134" s="6" t="s">
+      <c r="C136" s="6" t="s">
         <v>308</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C134">
-    <sortCondition ref="A2:A134"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D136">
+    <sortCondition ref="A2:A136"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="70fbc179-56b2-4609-9c4f-f2d8c8a53629">
@@ -3172,15 +3232,6 @@
     <TaxCatchAll xmlns="a1800618-4cc3-44a3-b2ff-4430b6f3c67d" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3385,20 +3436,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1D8E027-CFDE-468D-BB88-11F7DAD0A379}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6C0F10C-613D-4A36-8617-F7ABFFEFF28A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="70fbc179-56b2-4609-9c4f-f2d8c8a53629"/>
     <ds:schemaRef ds:uri="a1800618-4cc3-44a3-b2ff-4430b6f3c67d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1D8E027-CFDE-468D-BB88-11F7DAD0A379}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added grouped exposure calculations, implemented feedback from core team
</commit_message>
<xml_diff>
--- a/DEVELOPMENT/analysis/definitions/codelists/20250515_ADEPT_medicines.xlsx
+++ b/DEVELOPMENT/analysis/definitions/codelists/20250515_ADEPT_medicines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgamb\Documents\GitHub\ADEPT_obj1\DEVELOPMENT\analysis\definitions\codelists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4410BE6-6226-4410-8705-438B467C9B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83A4D28-6FC2-4A94-BE8B-3FA6DA117A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4080" windowWidth="23040" windowHeight="9504" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MEDICINES_Obj_1&amp;2" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="405">
   <si>
     <t>Drug_abbreviation</t>
   </si>
@@ -1242,6 +1242,15 @@
   </si>
   <si>
     <t>N06AA</t>
+  </si>
+  <si>
+    <t>N06AF01</t>
+  </si>
+  <si>
+    <t>DP_ISOCARBOXAZID</t>
+  </si>
+  <si>
+    <t>Isocarboxazid</t>
   </si>
 </sst>
 </file>
@@ -1282,12 +1291,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1296,14 +1299,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF242424"/>
-      <name val="Aptos Narrow"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF242424"/>
       <name val="Aptos Narrow"/>
-      <charset val="1"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1335,7 +1346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1349,11 +1360,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1692,10 +1704,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:D136"/>
+  <dimension ref="A1:D137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="B142" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1706,13 +1718,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1921,7 +1933,7 @@
       <c r="B20" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="8" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1932,7 +1944,7 @@
       <c r="B21" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="8" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1943,7 +1955,7 @@
       <c r="B22" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="8" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1954,7 +1966,7 @@
       <c r="B23" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="8" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2061,10 +2073,10 @@
       <c r="A33" s="9" t="s">
         <v>393</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="10" t="s">
         <v>394</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="10" t="s">
         <v>395</v>
       </c>
     </row>
@@ -2091,13 +2103,13 @@
       </c>
     </row>
     <row r="36" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="10" t="s">
+      <c r="A36" s="9" t="s">
         <v>396</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="10" t="s">
         <v>397</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="9" t="s">
         <v>398</v>
       </c>
       <c r="D36"/>
@@ -2422,793 +2434,804 @@
       </c>
     </row>
     <row r="66" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="4" t="s">
-        <v>180</v>
+      <c r="A66" s="11" t="s">
+        <v>403</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>182</v>
+        <v>404</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="67" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="68" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="69" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B70" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="C70" s="4" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="70" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="6" t="s">
+    <row r="71" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B71" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="C71" s="4" t="s">
         <v>365</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>352</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="72" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
-        <v>327</v>
+        <v>351</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>328</v>
+        <v>352</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>329</v>
+        <v>353</v>
       </c>
     </row>
     <row r="73" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B74" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="C74" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="74" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="6" t="s">
+    <row r="75" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B75" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C74" s="6" t="s">
+      <c r="C75" s="6" t="s">
         <v>203</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="4" t="s">
-        <v>336</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="76" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B77" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="C76" s="4" t="s">
+      <c r="C77" s="4" t="s">
         <v>383</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="78" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>193</v>
+        <v>189</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>190</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="79" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
     </row>
     <row r="80" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="81" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="6" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="82" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="B82" s="6" t="s">
+      <c r="B83" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="C82" s="6" t="s">
+      <c r="C83" s="6" t="s">
         <v>161</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="C83" s="6" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="84" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B85" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="C84" s="4" t="s">
+      <c r="C85" s="4" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="85" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="6" t="s">
+    <row r="86" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B86" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C85" s="6" t="s">
+      <c r="C86" s="6" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="C86" s="4" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="87" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B88" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="C87" s="4" t="s">
+      <c r="C88" s="4" t="s">
         <v>386</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="C88" s="4" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="89" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B90" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="C89" s="6" t="s">
+      <c r="C90" s="6" t="s">
         <v>317</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="4" t="s">
-        <v>369</v>
-      </c>
-      <c r="B90" s="4" t="s">
-        <v>370</v>
-      </c>
-      <c r="C90" s="4" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="91" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
-        <v>318</v>
+        <v>369</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>319</v>
+        <v>370</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>320</v>
+        <v>371</v>
       </c>
     </row>
     <row r="92" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B93" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="C92" s="4" t="s">
+      <c r="C93" s="4" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="93" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="6" t="s">
+    <row r="94" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B94" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C93" s="6" t="s">
+      <c r="C94" s="6" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="B94" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="C94" s="4" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="95" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B96" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C95" s="6" t="s">
+      <c r="C96" s="6" t="s">
         <v>179</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="B96" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="C96" s="4" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="97" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="B97" s="6" t="s">
+      <c r="B98" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="C97" s="6" t="s">
+      <c r="C98" s="6" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="98" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="4" t="s">
+    <row r="99" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="B99" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="C98" s="6" t="s">
+      <c r="C99" s="6" t="s">
         <v>218</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="B99" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="C99" s="6" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="100" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="6" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="101" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="102" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="103" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="6" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="104" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="6" t="s">
-        <v>255</v>
+        <v>231</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>257</v>
+        <v>233</v>
       </c>
     </row>
     <row r="105" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="C105" s="6" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="B106" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="C105" s="4" t="s">
+      <c r="C106" s="4" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="106" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="4" t="s">
+    <row r="107" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B106" s="4" t="s">
+      <c r="B107" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C106" s="4" t="s">
+      <c r="C107" s="4" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="B107" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="C107" s="6" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="108" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C108" s="6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="B109" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C108" s="6" t="s">
+      <c r="C109" s="6" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="109" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="4" t="s">
+    <row r="110" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="B109" s="4" t="s">
+      <c r="B110" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="C109" s="4" t="s">
+      <c r="C110" s="4" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="110" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="6" t="s">
+    <row r="111" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="B110" s="4" t="s">
+      <c r="B111" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="C110" s="6" t="s">
+      <c r="C111" s="6" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="111" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="4" t="s">
+    <row r="112" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="B111" s="4" t="s">
+      <c r="B112" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C111" s="6" t="s">
+      <c r="C112" s="6" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="112" spans="1:3" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="6" t="s">
+    <row r="113" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="B112" s="4" t="s">
+      <c r="B113" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C112" s="6" t="s">
+      <c r="C113" s="6" t="s">
         <v>248</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="B113" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="C113" s="6" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="114" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="115" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="4" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="116" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="117" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="4" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="118" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B119" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="C118" s="6" t="s">
+      <c r="C119" s="6" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="119" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="6" t="s">
+    <row r="120" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="B119" s="4" t="s">
+      <c r="B120" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="C119" s="6" t="s">
+      <c r="C120" s="6" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="120" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="4" t="s">
+    <row r="121" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="B120" s="4" t="s">
+      <c r="B121" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="C120" s="6" t="s">
+      <c r="C121" s="6" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="10" t="s">
+      <c r="D121"/>
+    </row>
+    <row r="122" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="9" t="s">
         <v>399</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B122" s="10" t="s">
         <v>400</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C122" s="10" t="s">
         <v>401</v>
-      </c>
-      <c r="D121"/>
-    </row>
-    <row r="122" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="4" t="s">
-        <v>390</v>
-      </c>
-      <c r="B122" s="4" t="s">
-        <v>391</v>
-      </c>
-      <c r="C122" s="4" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="123" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="4" t="s">
-        <v>282</v>
+        <v>390</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="C123" s="6" t="s">
-        <v>284</v>
+        <v>391</v>
+      </c>
+      <c r="C123" s="4" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="124" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="4" t="s">
-        <v>165</v>
+        <v>282</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C124" s="4" t="s">
-        <v>167</v>
+        <v>283</v>
+      </c>
+      <c r="C124" s="6" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="125" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="4" t="s">
-        <v>285</v>
+        <v>165</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="C125" s="6" t="s">
-        <v>287</v>
+        <v>166</v>
+      </c>
+      <c r="C125" s="4" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="126" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="4" t="s">
-        <v>372</v>
+        <v>285</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>373</v>
-      </c>
-      <c r="C126" s="4" t="s">
-        <v>374</v>
+        <v>286</v>
+      </c>
+      <c r="C126" s="6" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="127" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="4" t="s">
-        <v>288</v>
+        <v>372</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="C127" s="6" t="s">
-        <v>290</v>
+        <v>373</v>
+      </c>
+      <c r="C127" s="4" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="128" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="B128" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C128" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="B128" s="4" t="s">
+      <c r="B129" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="C128" s="6" t="s">
+      <c r="C129" s="6" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="129" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="6" t="s">
+    <row r="130" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="B129" s="4" t="s">
+      <c r="B130" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="C129" s="6" t="s">
+      <c r="C130" s="6" t="s">
         <v>296</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="B130" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="C130" s="4" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="131" spans="1:4" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="C131" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A132" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="B131" s="4" t="s">
+      <c r="B132" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="C131" s="4" t="s">
+      <c r="C132" s="4" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A132" s="6" t="s">
+      <c r="D132" s="1"/>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A133" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="B132" s="4" t="s">
+      <c r="B133" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="C132" s="6" t="s">
+      <c r="C133" s="6" t="s">
         <v>302</v>
-      </c>
-      <c r="D132" s="1"/>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A133" s="4" t="s">
-        <v>375</v>
-      </c>
-      <c r="B133" s="4" t="s">
-        <v>376</v>
-      </c>
-      <c r="C133" s="4" t="s">
-        <v>377</v>
       </c>
       <c r="D133" s="1"/>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="B134" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="C134" s="4" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A135" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="B134" s="4" t="s">
+      <c r="B135" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="C134" s="4" t="s">
+      <c r="C135" s="4" t="s">
         <v>380</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A135" s="6" t="s">
-        <v>303</v>
-      </c>
-      <c r="B135" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="C135" s="6" t="s">
-        <v>305</v>
       </c>
       <c r="D135" s="1"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="B136" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="C136" s="6" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A137" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="B136" s="4" t="s">
+      <c r="B137" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="C136" s="6" t="s">
+      <c r="C137" s="6" t="s">
         <v>308</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D136">
-    <sortCondition ref="A2:A136"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C137">
+    <sortCondition ref="A137"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3224,17 +3247,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="70fbc179-56b2-4609-9c4f-f2d8c8a53629">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a1800618-4cc3-44a3-b2ff-4430b6f3c67d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007D26C639087F6D45ADFC3EC21F1D3A6E" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="878129f2fcc6ee12aa7a3f6919ba358e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="70fbc179-56b2-4609-9c4f-f2d8c8a53629" xmlns:ns3="a1800618-4cc3-44a3-b2ff-4430b6f3c67d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f17d72d02eee5b7172274046075b6715" ns2:_="" ns3:_="">
     <xsd:import namespace="70fbc179-56b2-4609-9c4f-f2d8c8a53629"/>
@@ -3435,6 +3447,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="70fbc179-56b2-4609-9c4f-f2d8c8a53629">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a1800618-4cc3-44a3-b2ff-4430b6f3c67d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1D8E027-CFDE-468D-BB88-11F7DAD0A379}">
   <ds:schemaRefs>
@@ -3444,17 +3467,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6C0F10C-613D-4A36-8617-F7ABFFEFF28A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="70fbc179-56b2-4609-9c4f-f2d8c8a53629"/>
-    <ds:schemaRef ds:uri="a1800618-4cc3-44a3-b2ff-4430b6f3c67d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5369F11-F0AC-4D42-9BDF-B8922C622A3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3471,4 +3483,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6C0F10C-613D-4A36-8617-F7ABFFEFF28A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="70fbc179-56b2-4609-9c4f-f2d8c8a53629"/>
+    <ds:schemaRef ds:uri="a1800618-4cc3-44a3-b2ff-4430b6f3c67d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>